<commit_message>
Fixed OSD335x power estimation to use worst-case scenario.
</commit_message>
<xml_diff>
--- a/DOCS/Power_Budget.xlsx
+++ b/DOCS/Power_Budget.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="OSD335-X Power Rails" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
   <si>
     <t>OSD335x-SM Family Power Budget</t>
   </si>
@@ -164,25 +164,10 @@
     <t>WORST CASE TOTAL PWR</t>
   </si>
   <si>
-    <t>1.03W</t>
-  </si>
-  <si>
     <t>WORST CASE EFFICIENCY LDO</t>
   </si>
   <si>
-    <t>0.206 A</t>
-  </si>
-  <si>
-    <t>82% (approx.) at 0.206A</t>
-  </si>
-  <si>
     <t>WORST CASE INPUT CURRENT</t>
-  </si>
-  <si>
-    <t>0.251 A</t>
-  </si>
-  <si>
-    <t>0.206/0.82</t>
   </si>
   <si>
     <t>NOTE:  If load current changes, use table from PMIC datasheet.</t>
@@ -236,6 +221,9 @@
   </si>
   <si>
     <t>Ethernet</t>
+  </si>
+  <si>
+    <t>1.53552150246105 W</t>
   </si>
 </sst>
 </file>
@@ -330,13 +318,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -347,6 +329,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -674,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,59 +685,59 @@
       <c r="J1" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>4.3</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>5</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>5.8</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <v>2</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H6" t="s">
@@ -757,362 +745,354 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>4.3</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>5</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>5.8</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>1.3</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>2.75</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <v>3.7</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>5.5</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <v>2</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="6">
         <v>3.4</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="D12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="6">
         <v>0.5</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="6">
         <v>3.3</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="D13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="6">
         <v>0.5</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="8">
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="6">
         <v>3.3</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="D14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="6">
         <v>0.1</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="8">
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="6">
         <v>1.8</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="8">
+      <c r="D15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="6">
         <v>0.05</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="6">
         <v>1.8</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="D16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="6">
         <v>0.1</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="8">
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="6">
         <v>1.8</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="D17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="6">
         <v>0.25</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="8">
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="6">
         <v>1.5</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="D18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="8">
+      <c r="B19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="D19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="8">
+      <c r="B20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="8" t="s">
+      <c r="D20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="8">
+      <c r="B21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="6">
         <v>1.8</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="D21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="E28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="E29" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="E28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1131,7 +1111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -1143,37 +1123,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -1183,178 +1163,178 @@
       <c r="E4" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A22:E22"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added internal PMIC, LDO datasheets and reference design.
</commit_message>
<xml_diff>
--- a/DOCS/Power_Budget.xlsx
+++ b/DOCS/Power_Budget.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\ele682\DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\club\Desktop\Dossier des membres\Ben\Git\ele682\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OSD335-X Power Rails" sheetId="1" r:id="rId1"/>
     <sheet name="Peripheral Power Consumption" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Power Budget" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="81">
   <si>
     <t>OSD335x-SM Family Power Budget</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>Power Estimation Tool</t>
-  </si>
-  <si>
-    <t>WORST CASE TOTAL PWR</t>
   </si>
   <si>
     <t>WORST CASE EFFICIENCY LDO</t>
@@ -205,9 +202,6 @@
     <t>Current Consumption (typ)</t>
   </si>
   <si>
-    <t>Current Peaks (max)</t>
-  </si>
-  <si>
     <t>USB</t>
   </si>
   <si>
@@ -223,13 +217,87 @@
     <t>Ethernet</t>
   </si>
   <si>
-    <t>1.53552150246105 W</t>
+    <t>WORST CASE TOTAL PWR (W)</t>
+  </si>
+  <si>
+    <t>AM335x</t>
+  </si>
+  <si>
+    <t>Processor</t>
+  </si>
+  <si>
+    <t>Supply Voltage</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Max Power (mW)</t>
+  </si>
+  <si>
+    <t>Used worst case scenario, all processing at maximum.
+Typical usage should be much less.
+Inrush current when powered on is estimated at 1.5A using VIN_AC and 0,5A using VIN_USB.</t>
+  </si>
+  <si>
+    <t>Operating Voltage (typ) (V)</t>
+  </si>
+  <si>
+    <t>DDR RAM</t>
+  </si>
+  <si>
+    <t>DDR/RAM</t>
+  </si>
+  <si>
+    <t>Max Current (A)</t>
+  </si>
+  <si>
+    <t>PMIC</t>
+  </si>
+  <si>
+    <t>TPS65217</t>
+  </si>
+  <si>
+    <t>Used values stipulated in Power Budget example from Octavo systems.</t>
+  </si>
+  <si>
+    <t>Less than 5</t>
+  </si>
+  <si>
+    <t>Less than 0,001</t>
+  </si>
+  <si>
+    <t>Negligeable.  Used values in Power Budget example from Octavo systems.</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>TL5209</t>
+  </si>
+  <si>
+    <t>Maximum quiescent current when Ven is greater than 3V and maximum load (500mA).</t>
+  </si>
+  <si>
+    <t>Voltage Rail</t>
+  </si>
+  <si>
+    <t>Peripherals</t>
+  </si>
+  <si>
+    <t>Peripheral Max Current</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Max Supported Current (A)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -309,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -331,11 +399,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -398,7 +478,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -662,11 +742,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
@@ -685,15 +765,15 @@
       <c r="J1" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -791,15 +871,15 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1060,39 +1140,39 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B27" s="12">
+        <v>1.53552150246105</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="E29" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1109,232 +1189,469 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="E15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="E19" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="E23" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="14">
+        <v>5</v>
+      </c>
+      <c r="E28" s="14">
+        <v>1540</v>
+      </c>
+      <c r="F28" s="14">
+        <v>0.308</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="E32" s="14">
+        <v>508.5</v>
+      </c>
+      <c r="F32" s="14">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B36" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="14">
+        <v>5</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="14">
+        <v>5</v>
+      </c>
+      <c r="E40" s="14">
+        <v>125</v>
+      </c>
+      <c r="F40" s="14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A18:E18"/>
+  <mergeCells count="10">
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1342,12 +1659,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C2:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added datasheets for serial, HDMI, processor, and WIFI module.
</commit_message>
<xml_diff>
--- a/DOCS/Power_Budget.xlsx
+++ b/DOCS/Power_Budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\club\Desktop\Dossier des membres\Ben\Git\ele682\DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\ele682\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Peripheral Power Consumption" sheetId="2" r:id="rId2"/>
     <sheet name="Power Budget" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="93">
   <si>
     <t>OSD335x-SM Family Power Budget</t>
   </si>
@@ -202,12 +202,6 @@
     <t>Current Consumption (typ)</t>
   </si>
   <si>
-    <t>USB</t>
-  </si>
-  <si>
-    <t>Serial</t>
-  </si>
-  <si>
     <t>Wifi</t>
   </si>
   <si>
@@ -292,12 +286,55 @@
   </si>
   <si>
     <t>Max Supported Current (A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDA19988 </t>
+  </si>
+  <si>
+    <t>1.8V</t>
+  </si>
+  <si>
+    <t>Max power consumption when running in full speed mode.
+NOTE: On Octavo example, says this chip is 385mW max, which would mean 0.215A.</t>
+  </si>
+  <si>
+    <t>0.5 per port</t>
+  </si>
+  <si>
+    <t>USB standard allows a device to draw 500mA max on port.</t>
+  </si>
+  <si>
+    <t>2500 per port (host)</t>
+  </si>
+  <si>
+    <t>8.3mA in normal operating condition.</t>
+  </si>
+  <si>
+    <t>FT230X</t>
+  </si>
+  <si>
+    <t>USB (AS HOST)</t>
+  </si>
+  <si>
+    <t>Serial (AS USB DEVICE TOO?)</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>WF111A</t>
+  </si>
+  <si>
+    <t>250 mA in peak tx, 190 mA typical (+16dBm)</t>
+  </si>
+  <si>
+    <t>3.3V, some pins 1.8V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -402,12 +439,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -416,6 +447,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,7 +527,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -746,7 +795,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
@@ -765,15 +814,15 @@
       <c r="J1" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -871,15 +920,15 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1140,17 +1189,17 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="12">
+        <v>54</v>
+      </c>
+      <c r="B27" s="10">
         <v>1.53552150246105</v>
       </c>
       <c r="C27" s="3"/>
@@ -1191,41 +1240,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="54.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>50</v>
@@ -1234,13 +1284,23 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+    <row r="3" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="16">
+        <v>207</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.115</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -1251,27 +1311,27 @@
       <c r="G4" s="2"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="B6" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>50</v>
@@ -1282,34 +1342,42 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15">
+        <v>5</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="B10" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>50</v>
@@ -1319,35 +1387,45 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
+      <c r="B12" s="15" t="s">
+        <v>86</v>
+      </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="D12" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="15">
+        <v>41.5</v>
+      </c>
+      <c r="F12" s="15">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="B14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>50</v>
@@ -1357,35 +1435,45 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
+      <c r="B16" s="15" t="s">
+        <v>90</v>
+      </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="D16" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="15">
+        <v>825</v>
+      </c>
+      <c r="F16" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="B18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>50</v>
@@ -1403,27 +1491,27 @@
       <c r="G20" s="3"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="B22" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>50</v>
@@ -1441,219 +1529,220 @@
       <c r="G24" s="4"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="B26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="F27" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="14" t="s">
+      <c r="B28" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="12">
+        <v>5</v>
+      </c>
+      <c r="E28" s="12">
+        <v>1540</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0.308</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="14">
-        <v>5</v>
-      </c>
-      <c r="E28" s="14">
-        <v>1540</v>
-      </c>
-      <c r="F28" s="14">
-        <v>0.308</v>
-      </c>
-      <c r="G28" s="13" t="s">
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="F31" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="E32" s="12">
+        <v>508.5</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="E32" s="14">
-        <v>508.5</v>
-      </c>
-      <c r="F32" s="14">
-        <v>0.33900000000000002</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C35" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="F35" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G35" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="12">
+        <v>5</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="14">
-        <v>5</v>
-      </c>
-      <c r="E36" s="14" t="s">
+      <c r="F36" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="14" t="s">
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G36" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C39" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="F39" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="14">
+      <c r="B40" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="12">
         <v>5</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="12">
         <v>125</v>
       </c>
-      <c r="F40" s="14">
+      <c r="F40" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G40" s="13" t="s">
-        <v>75</v>
+      <c r="G40" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B18:G18"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1665,7 +1754,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
@@ -1676,19 +1765,19 @@
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
         <v>76</v>
       </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>77</v>
-      </c>
-      <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Prep pwr budget for report
</commit_message>
<xml_diff>
--- a/DOCS/Power_Budget.xlsx
+++ b/DOCS/Power_Budget.xlsx
@@ -1,32 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\ele682\DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\ETS\Hivers 2020\ELE682\ele682\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8863EF7-6661-4BE2-8490-E5F8A710E06D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="7448" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OSD335-X Power Rails" sheetId="1" r:id="rId1"/>
     <sheet name="Peripheral Power Consumption" sheetId="2" r:id="rId2"/>
     <sheet name="Power Budget" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="124">
   <si>
     <t>OSD335x-SM Family Power Budget</t>
   </si>
@@ -273,15 +279,6 @@
     <t>Maximum quiescent current when Ven is greater than 3V and maximum load (500mA).</t>
   </si>
   <si>
-    <t>Voltage Rail</t>
-  </si>
-  <si>
-    <t>Peripherals</t>
-  </si>
-  <si>
-    <t>Max Supported Current (A)</t>
-  </si>
-  <si>
     <t xml:space="preserve">TDA19988 </t>
   </si>
   <si>
@@ -328,42 +325,15 @@
     <t>DDR</t>
   </si>
   <si>
-    <t>Efficiency</t>
-  </si>
-  <si>
-    <t>Peripheral Max Power at Operating Voltage (mW)</t>
-  </si>
-  <si>
-    <t>Voltage (V)</t>
-  </si>
-  <si>
-    <t>Max Power at Rail (mW)</t>
-  </si>
-  <si>
-    <t>Current at Rail (A)</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Efficiency*</t>
-  </si>
-  <si>
     <t>*Efficiency measures taken at worst case load.</t>
   </si>
   <si>
-    <t>Will be modified when power budget is complete.</t>
-  </si>
-  <si>
     <t>SYS_VOUT</t>
   </si>
   <si>
-    <t>Ethernet*</t>
-  </si>
-  <si>
-    <t>*Ethernet is here because max supply for PHY is 3.47, better to place it on a 3.3V rail.</t>
-  </si>
-  <si>
     <t>HDMI Pwr</t>
   </si>
   <si>
@@ -380,13 +350,99 @@
   </si>
   <si>
     <t>3.3V</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"HDMI sink shall not sink more than 55mA." - TI app note snva412c </t>
+  </si>
+  <si>
+    <t>RTC power consumption already calculated in processor.</t>
+  </si>
+  <si>
+    <t>Efficiency set to 1 since SYS is the input voltage switched.  Good estimation.</t>
+  </si>
+  <si>
+    <t>According to Toshiba micro memory card specs, 80mA max draw.  MMC power consumption already counted on processor power consumption.</t>
+  </si>
+  <si>
+    <t>Ethernet PHY</t>
+  </si>
+  <si>
+    <t>HDMI Transceiver</t>
+  </si>
+  <si>
+    <t>Reset Buffer</t>
+  </si>
+  <si>
+    <t>Uart-to-USB</t>
+  </si>
+  <si>
+    <t>TPS2051</t>
+  </si>
+  <si>
+    <t>USB hub IC</t>
+  </si>
+  <si>
+    <t>110mA max current draw when two HS devices are connected to the hub.</t>
+  </si>
+  <si>
+    <t>Tension (V)</t>
+  </si>
+  <si>
+    <t>Courant maximal (A)</t>
+  </si>
+  <si>
+    <t>Périphériques</t>
+  </si>
+  <si>
+    <t>Efficacité*</t>
+  </si>
+  <si>
+    <t>Rail d'alimentation</t>
+  </si>
+  <si>
+    <t>PUISSANCE CONSOMMÉE MAXIMALE</t>
+  </si>
+  <si>
+    <t>Puissance (mW)</t>
+  </si>
+  <si>
+    <t>Courant (A)</t>
+  </si>
+  <si>
+    <t>HDMI Video 
+Clock Generator</t>
+  </si>
+  <si>
+    <t>HDMI Audio
+lock Generator</t>
+  </si>
+  <si>
+    <t>P max sur 
+le rail (mW)</t>
+  </si>
+  <si>
+    <t>P max des 
+périphériques (mW)</t>
+  </si>
+  <si>
+    <t>Courant 
+sur le rail (A)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,6 +453,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -429,7 +500,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -535,11 +606,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -585,50 +687,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,7 +813,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -952,43 +1107,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.73046875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1011,7 +1166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1060,7 +1215,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1083,18 +1238,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1295,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1163,7 +1318,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1186,7 +1341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1209,7 +1364,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -1232,7 +1387,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1255,7 +1410,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1278,7 +1433,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -1301,7 +1456,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1324,7 +1479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
@@ -1347,19 +1502,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="G23" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
@@ -1368,7 +1523,7 @@
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
@@ -1378,7 +1533,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
@@ -1401,34 +1556,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G40"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>48</v>
       </c>
@@ -1448,9 +1603,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B3" s="14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="14">
@@ -1463,16 +1618,16 @@
         <v>0.115</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="13" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="13" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E4" s="13">
         <v>250</v>
@@ -1481,20 +1636,20 @@
         <v>0.05</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B6" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
@@ -1514,33 +1669,33 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" s="2"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13">
         <v>5</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B10" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>48</v>
       </c>
@@ -1560,13 +1715,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E12" s="13">
         <v>41.5</v>
@@ -1575,20 +1730,20 @@
         <v>8.3000000000000001E-3</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B14" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
@@ -1608,13 +1763,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E16" s="13">
         <v>825</v>
@@ -1623,20 +1778,20 @@
         <v>0.25</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B18" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
         <v>48</v>
       </c>
@@ -1656,7 +1811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B20" s="2"/>
       <c r="C20" s="8"/>
       <c r="D20" s="2"/>
@@ -1664,17 +1819,17 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B22" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
         <v>48</v>
       </c>
@@ -1694,33 +1849,33 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="19">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B24" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="17">
         <v>393</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="17">
         <v>0.11899999999999999</v>
       </c>
-      <c r="G24" s="19"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="18" t="s">
+      <c r="G24" s="17"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B26" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B27" s="8" t="s">
         <v>48</v>
       </c>
@@ -1740,7 +1895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="57" x14ac:dyDescent="0.45">
       <c r="B28" s="11" t="s">
         <v>55</v>
       </c>
@@ -1760,17 +1915,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="18" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B30" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B31" s="8" t="s">
         <v>48</v>
       </c>
@@ -1790,7 +1945,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B32" s="11" t="s">
         <v>63</v>
       </c>
@@ -1810,17 +1965,17 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="s">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B34" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B35" s="8" t="s">
         <v>48</v>
       </c>
@@ -1840,7 +1995,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B36" s="11" t="s">
         <v>66</v>
       </c>
@@ -1860,17 +2015,17 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="18" t="s">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B38" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B39" s="8" t="s">
         <v>48</v>
       </c>
@@ -1890,7 +2045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B40" s="11" t="s">
         <v>72</v>
       </c>
@@ -1929,796 +2084,887 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:L49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.59765625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.46484375" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.46484375" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="130.3984375" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.86328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1328125" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C2" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="12" t="s">
+    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="24">
+        <v>5</v>
+      </c>
+      <c r="C3" s="24">
+        <v>2</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="25">
+        <v>1540</v>
+      </c>
+      <c r="F3" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="G3" s="26">
+        <f>E3/$F$3</f>
+        <v>1621.0526315789475</v>
+      </c>
+      <c r="H3" s="26">
+        <f>(G3/$B$3)/1000</f>
+        <v>0.3242105263157895</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="25">
+        <v>5</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="G4" s="26">
+        <f t="shared" ref="G4:G6" si="0">E4/$F$3</f>
+        <v>5.2631578947368425</v>
+      </c>
+      <c r="H4" s="26">
+        <f t="shared" ref="H4:H6" si="1">(G4/$B$3)/1000</f>
+        <v>1.0526315789473686E-3</v>
+      </c>
+      <c r="I4" s="30"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="25">
+        <v>125</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="26">
+        <f t="shared" si="0"/>
+        <v>131.57894736842107</v>
+      </c>
+      <c r="H5" s="26">
+        <f t="shared" si="1"/>
+        <v>2.6315789473684213E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="25">
+        <v>508.5</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="26">
+        <f t="shared" si="0"/>
+        <v>535.26315789473688</v>
+      </c>
+      <c r="H6" s="26">
+        <f t="shared" si="1"/>
+        <v>0.10705263157894737</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="32"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36">
+        <f>SUM(G3:G6)</f>
+        <v>2293.1578947368425</v>
+      </c>
+      <c r="H7" s="36">
+        <f>SUM(H3:H6)</f>
+        <v>0.4586315789473685</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="24">
+        <v>5</v>
+      </c>
+      <c r="C10" s="24">
+        <v>1.3</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="25">
+        <v>1540</v>
+      </c>
+      <c r="F10" s="37">
+        <v>0.95</v>
+      </c>
+      <c r="G10" s="26">
+        <f>E10/$F$10</f>
+        <v>1621.0526315789475</v>
+      </c>
+      <c r="H10" s="26">
+        <f>(G10/$B$10)/1000</f>
+        <v>0.3242105263157895</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="25">
+        <v>5</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="26">
+        <f t="shared" ref="G11:G14" si="2">E11/$F$10</f>
+        <v>5.2631578947368425</v>
+      </c>
+      <c r="H11" s="26">
+        <f t="shared" ref="H11:H14" si="3">(G11/$B$10)/1000</f>
+        <v>1.0526315789473686E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="25">
+        <v>125</v>
+      </c>
+      <c r="F12" s="38"/>
+      <c r="G12" s="26">
+        <f t="shared" si="2"/>
+        <v>131.57894736842107</v>
+      </c>
+      <c r="H12" s="26">
+        <f t="shared" si="3"/>
+        <v>2.6315789473684213E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="25">
+        <v>508.5</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="26">
+        <f t="shared" si="2"/>
+        <v>535.26315789473688</v>
+      </c>
+      <c r="H13" s="26">
+        <f t="shared" si="3"/>
+        <v>0.10705263157894737</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="25">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F14" s="39"/>
+      <c r="G14" s="26">
+        <f t="shared" si="2"/>
+        <v>4.3684210526315796</v>
+      </c>
+      <c r="H14" s="26">
+        <f t="shared" si="3"/>
+        <v>8.73684210526316E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="32"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="36">
+        <f>SUM(G10:G14)</f>
+        <v>2297.5263157894742</v>
+      </c>
+      <c r="H15" s="36">
+        <f>SUM(H10:H14)</f>
+        <v>0.45950526315789481</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24">
+        <v>3.4</v>
+      </c>
+      <c r="C18" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="25">
+        <v>0</v>
+      </c>
+      <c r="F18" s="40">
+        <v>0.92</v>
+      </c>
+      <c r="G18" s="26">
+        <f>E18/$F$18</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="26">
+        <f>(G18/$B$18)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="32"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="36">
+        <f>SUM(G18:G18)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="36">
+        <f>SUM(H18:H18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="24">
+        <v>3.3</v>
+      </c>
+      <c r="C22" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="25">
+        <v>393</v>
+      </c>
+      <c r="F22" s="24">
+        <v>0.92</v>
+      </c>
+      <c r="G22" s="26">
+        <f>E22/$F$22</f>
+        <v>427.17391304347825</v>
+      </c>
+      <c r="H22" s="26">
+        <f>(G22/$B$22)/1000</f>
+        <v>0.12944664031620554</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="25">
+        <v>264</v>
+      </c>
+      <c r="F23" s="29"/>
+      <c r="G23" s="26">
+        <f t="shared" ref="G23:G26" si="4">E23/$F$22</f>
+        <v>286.95652173913044</v>
+      </c>
+      <c r="H23" s="26">
+        <f t="shared" ref="H23:H26" si="5">(G23/$B$22)/1000</f>
+        <v>8.6956521739130432E-2</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="25">
+        <f>(0.015*3.3)*1000</f>
+        <v>49.499999999999993</v>
+      </c>
+      <c r="F24" s="29"/>
+      <c r="G24" s="26">
+        <f t="shared" si="4"/>
+        <v>53.804347826086946</v>
+      </c>
+      <c r="H24" s="26">
+        <f t="shared" si="5"/>
+        <v>1.6304347826086953E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="25">
+        <v>363</v>
+      </c>
+      <c r="F25" s="29"/>
+      <c r="G25" s="26">
+        <f t="shared" si="4"/>
+        <v>394.56521739130432</v>
+      </c>
+      <c r="H25" s="26">
+        <f t="shared" si="5"/>
+        <v>0.11956521739130434</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="25">
+        <v>49.5</v>
+      </c>
+      <c r="F26" s="31"/>
+      <c r="G26" s="26">
+        <f t="shared" si="4"/>
+        <v>53.804347826086953</v>
+      </c>
+      <c r="H26" s="26">
+        <f t="shared" si="5"/>
+        <v>1.6304347826086956E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="32"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="36">
+        <f>SUM(G22:G26)</f>
+        <v>1216.304347826087</v>
+      </c>
+      <c r="H27" s="36">
+        <f>SUM(H22:H26)</f>
+        <v>0.36857707509881421</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="24">
+        <v>1.8</v>
+      </c>
+      <c r="C30" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="25">
+        <v>207</v>
+      </c>
+      <c r="F30" s="40">
+        <v>0.84</v>
+      </c>
+      <c r="G30" s="26">
+        <f>E30/$F$30</f>
+        <v>246.42857142857144</v>
+      </c>
+      <c r="H30" s="26">
+        <f>(G30/$B$30)/1000</f>
+        <v>0.13690476190476189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="32"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36">
+        <f>SUM(G30:G30)</f>
+        <v>246.42857142857144</v>
+      </c>
+      <c r="H31" s="36">
+        <f>SUM(H30:H30)</f>
+        <v>0.13690476190476189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A33" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I33" s="42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="24">
+        <v>1.8</v>
+      </c>
+      <c r="C34" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="25">
+        <v>2</v>
+      </c>
+      <c r="F34" s="24">
+        <v>0.84</v>
+      </c>
+      <c r="G34" s="36">
+        <f>E34/$F$30</f>
+        <v>2.3809523809523809</v>
+      </c>
+      <c r="H34" s="43">
+        <f>(G34/$B$30)/1000</f>
+        <v>1.3227513227513229E-3</v>
+      </c>
+      <c r="I34" s="42"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="E35" s="25">
+        <v>0</v>
+      </c>
+      <c r="F35" s="31"/>
+      <c r="G35" s="26">
+        <f>E35/$F$30</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="26">
+        <f>(G35/$B$30)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="32"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="34"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="36">
+        <f>SUM(G35:G35)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="36">
+        <f>SUM(H35:H35)</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="25"/>
+    </row>
+    <row r="38" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A38" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="24">
+        <v>5</v>
+      </c>
+      <c r="C39" s="24">
+        <v>2</v>
+      </c>
+      <c r="D39" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C3" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="20">
-        <v>5</v>
-      </c>
-      <c r="E3" s="20">
-        <v>2</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="19">
-        <v>1540</v>
-      </c>
-      <c r="H3" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="I3" s="26">
-        <f>G3/$H$3</f>
-        <v>1711.1111111111111</v>
-      </c>
-      <c r="J3" s="26">
-        <f>(I3/$D$3)/1000</f>
-        <v>0.34222222222222221</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="E39" s="25">
+        <v>275</v>
+      </c>
+      <c r="F39" s="24">
+        <v>1</v>
+      </c>
+      <c r="G39" s="26">
+        <f>E39/$F$39</f>
+        <v>275</v>
+      </c>
+      <c r="H39" s="45">
+        <f>(G39/$B$39)/1000</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="I39" s="46" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="31"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="19">
-        <v>5</v>
-      </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="26">
-        <f t="shared" ref="I4:I6" si="0">G4/$H$3</f>
-        <v>5.5555555555555554</v>
-      </c>
-      <c r="J4" s="26">
-        <f t="shared" ref="J4:J6" si="1">(I4/$D$3)/1000</f>
-        <v>1.1111111111111111E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C5" s="31"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="19">
-        <v>125</v>
-      </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="26">
-        <f t="shared" si="0"/>
-        <v>138.88888888888889</v>
-      </c>
-      <c r="J5" s="26">
-        <f t="shared" si="1"/>
-        <v>2.777777777777778E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="31"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="G6" s="19">
-        <v>508.5</v>
-      </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="26">
-        <f t="shared" si="0"/>
-        <v>565</v>
-      </c>
-      <c r="J6" s="26">
-        <f t="shared" si="1"/>
-        <v>0.113</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="30"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="9">
-        <f>SUM(I3:I6)</f>
-        <v>2420.5555555555557</v>
-      </c>
-      <c r="J7" s="9">
-        <f>SUM(J3:J6)</f>
-        <v>0.4841111111111111</v>
-      </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C9" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C10" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="20">
-        <v>5</v>
-      </c>
-      <c r="E10" s="20">
-        <v>1.3</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G10" s="19">
-        <v>1540</v>
-      </c>
-      <c r="H10" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="I10" s="26">
-        <f>G10/$H$10</f>
-        <v>1711.1111111111111</v>
-      </c>
-      <c r="J10" s="26">
-        <f>(I10/$D$10)/1000</f>
-        <v>0.34222222222222221</v>
-      </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C11" s="31"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="19">
-        <v>5</v>
-      </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="26">
-        <f t="shared" ref="I11:I13" si="2">G11/$H$10</f>
-        <v>5.5555555555555554</v>
-      </c>
-      <c r="J11" s="26">
-        <f t="shared" ref="J11:J13" si="3">(I11/$D$10)/1000</f>
-        <v>1.1111111111111111E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C12" s="31"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="19">
-        <v>125</v>
-      </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="26">
-        <f t="shared" si="2"/>
-        <v>138.88888888888889</v>
-      </c>
-      <c r="J12" s="26">
-        <f t="shared" si="3"/>
-        <v>2.777777777777778E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C13" s="31"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="G13" s="19">
-        <v>508.5</v>
-      </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="26">
-        <f t="shared" si="2"/>
-        <v>565</v>
-      </c>
-      <c r="J13" s="26">
-        <f t="shared" si="3"/>
-        <v>0.113</v>
-      </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C14" s="30"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="9">
-        <f>SUM(I10:I13)</f>
-        <v>2420.5555555555557</v>
-      </c>
-      <c r="J14" s="9">
-        <f>SUM(J10:J13)</f>
-        <v>0.4841111111111111</v>
-      </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C16" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C17" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="20">
-        <v>3.4</v>
-      </c>
-      <c r="E17" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="I17" s="26">
-        <f>G17/$H$17</f>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="28"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="25"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="26">
+        <f t="shared" ref="G40" si="6">E40/$F$3</f>
         <v>0</v>
       </c>
-      <c r="J17" s="26">
-        <f>(I17/$D$17)/1000</f>
+      <c r="H40" s="26">
+        <f t="shared" ref="H40" si="7">(G40/$B$3)/1000</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C18" s="31"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="19">
-        <v>825</v>
-      </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="26">
-        <f t="shared" ref="I18:I20" si="4">G18/$H$17</f>
-        <v>916.66666666666663</v>
-      </c>
-      <c r="J18" s="26">
-        <f t="shared" ref="J18:J20" si="5">(I18/$D$17)/1000</f>
-        <v>0.26960784313725494</v>
-      </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C19" s="31"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="26">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C20" s="31"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="26">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="30"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="9">
-        <f>SUM(I17:I20)</f>
-        <v>916.66666666666663</v>
-      </c>
-      <c r="J21" s="9">
-        <f>SUM(J17:J20)</f>
-        <v>0.26960784313725494</v>
-      </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="20">
-        <v>3.3</v>
-      </c>
-      <c r="E24" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="F24" s="19" t="s">
+      <c r="I40" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="G24" s="19">
-        <v>393</v>
-      </c>
-      <c r="H24" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="I24" s="26">
-        <f>G24/$H$24</f>
-        <v>436.66666666666663</v>
-      </c>
-      <c r="J24" s="26">
-        <f>(I24/$D$24)/1000</f>
-        <v>0.13232323232323234</v>
-      </c>
-      <c r="L24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="31"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="26">
-        <f t="shared" ref="I25:I27" si="6">G25/$H$24</f>
-        <v>0</v>
-      </c>
-      <c r="J25" s="26">
-        <f t="shared" ref="J25:J27" si="7">(I25/$D$24)/1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C26" s="31"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="26">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="26">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="31"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="26">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="26">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="30"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="9">
-        <f>SUM(I24:I27)</f>
-        <v>436.66666666666663</v>
-      </c>
-      <c r="J28" s="9">
-        <f>SUM(J24:J27)</f>
-        <v>0.13232323232323234</v>
-      </c>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C30" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C31" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="20">
-        <v>1.8</v>
-      </c>
-      <c r="E31" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" s="19">
-        <v>207</v>
-      </c>
-      <c r="H31" s="28">
-        <v>0.9</v>
-      </c>
-      <c r="I31" s="26">
-        <f>G31/$H$31</f>
-        <v>230</v>
-      </c>
-      <c r="J31" s="26">
-        <f>(I31/$D$31)/1000</f>
-        <v>0.12777777777777777</v>
-      </c>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C32" s="30"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="G32" s="24"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="9">
-        <f>SUM(I31:I31)</f>
-        <v>230</v>
-      </c>
-      <c r="J32" s="9">
-        <f>SUM(J31:J31)</f>
-        <v>0.12777777777777777</v>
-      </c>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C42" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H42" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="I42" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="J42" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C43" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D43" s="20">
-        <v>5</v>
-      </c>
-      <c r="E43" s="20">
-        <v>2</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="G43" s="19">
-        <v>250</v>
-      </c>
-      <c r="H43" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="I43" s="26">
-        <f>G43/$H$43</f>
-        <v>277.77777777777777</v>
-      </c>
-      <c r="J43" s="26">
-        <f>(I43/$D$43)/1000</f>
-        <v>5.5555555555555559E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="26">
-        <f t="shared" ref="I44:I48" si="8">G44/$H$3</f>
-        <v>0</v>
-      </c>
-      <c r="J44" s="26">
-        <f t="shared" ref="J44:J48" si="9">(I44/$D$3)/1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J45" s="26">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J46" s="26">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J47" s="26">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J48" s="26">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="G49" s="24"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="9">
-        <f>SUM(I43:I48)</f>
-        <v>277.77777777777777</v>
-      </c>
-      <c r="J49" s="9">
-        <f>SUM(J43:J48)</f>
-        <v>5.5555555555555559E-2</v>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="32"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E41" s="34"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="36">
+        <f>SUM(G39:G40)</f>
+        <v>275</v>
+      </c>
+      <c r="H41" s="36">
+        <f>SUM(H39:H40)</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="I41" s="46"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F46" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="G46" s="47"/>
+      <c r="H46" s="47"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F47" s="25"/>
+      <c r="G47" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="H47" s="48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F48" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="G48" s="26">
+        <f>SUM(G15,G19,G27,G31,G41)</f>
+        <v>4035.2592350441328</v>
+      </c>
+      <c r="H48" s="25">
+        <f>(G48/5)/1000</f>
+        <v>0.80705184700882659</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="D43:D49"/>
-    <mergeCell ref="E43:E49"/>
-    <mergeCell ref="H43:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="E17:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="H17:H20"/>
+  <mergeCells count="34">
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
     <mergeCell ref="C3:C7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="E10:E14"/>
-    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update pwr budget and rapport prelim
</commit_message>
<xml_diff>
--- a/DOCS/Power_Budget.xlsx
+++ b/DOCS/Power_Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\ETS\Hivers 2020\ELE682\ele682\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8863EF7-6661-4BE2-8490-E5F8A710E06D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8662FDC0-6B43-4E21-BBAF-01775575C4C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="7448" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="123">
   <si>
     <t>OSD335x-SM Family Power Budget</t>
   </si>
@@ -355,9 +355,6 @@
     <t>RTC</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t xml:space="preserve">"HDMI sink shall not sink more than 55mA." - TI app note snva412c </t>
   </si>
   <si>
@@ -401,9 +398,6 @@
   </si>
   <si>
     <t>Efficacité*</t>
-  </si>
-  <si>
-    <t>Rail d'alimentation</t>
   </si>
   <si>
     <t>PUISSANCE CONSOMMÉE MAXIMALE</t>
@@ -433,14 +427,18 @@
   <si>
     <t>Courant 
 sur le rail (A)</t>
+  </si>
+  <si>
+    <t>Alimentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -690,12 +688,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -703,67 +695,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -775,6 +728,51 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1111,7 +1109,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A5" sqref="A5:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1133,15 +1131,15 @@
       <c r="J1" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
@@ -1239,15 +1237,15 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
@@ -1508,11 +1506,11 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
@@ -1559,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -1574,14 +1572,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
@@ -1640,14 +1638,14 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
@@ -1686,14 +1684,14 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
@@ -1734,14 +1732,14 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
@@ -1782,14 +1780,14 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
@@ -1820,14 +1818,14 @@
       <c r="G20" s="2"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
@@ -1866,14 +1864,14 @@
       <c r="G24" s="17"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B27" s="8" t="s">
@@ -1916,14 +1914,14 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B31" s="8" t="s">
@@ -1966,14 +1964,14 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B35" s="8" t="s">
@@ -2016,14 +2014,14 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B39" s="8" t="s">
@@ -2085,888 +2083,755 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:I48"/>
+  <dimension ref="A2:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H7"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.53125" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.46484375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.46484375" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.265625" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="130.3984375" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.86328125" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1328125" style="22"/>
+    <col min="1" max="1" width="12.1328125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.46484375" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.46484375" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="130.3984375" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.86328125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1328125" style="20"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="20" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="38">
         <v>5</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="38">
         <v>2</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="21">
         <v>1540</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="38">
         <v>0.95</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="22">
         <f>E3/$F$3</f>
         <v>1621.0526315789475</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="22">
         <f>(G3/$B$3)/1000</f>
         <v>0.3242105263157895</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="23" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="25" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="21">
         <v>5</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="26">
+      <c r="F4" s="47"/>
+      <c r="G4" s="22">
         <f t="shared" ref="G4:G6" si="0">E4/$F$3</f>
         <v>5.2631578947368425</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="22">
         <f t="shared" ref="H4:H6" si="1">(G4/$B$3)/1000</f>
         <v>1.0526315789473686E-3</v>
       </c>
-      <c r="I4" s="30"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="25" t="s">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="21">
         <v>125</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="26">
+      <c r="F5" s="47"/>
+      <c r="G5" s="22">
         <f t="shared" si="0"/>
         <v>131.57894736842107</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="22">
         <f t="shared" si="1"/>
         <v>2.6315789473684213E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="25" t="s">
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="21">
         <v>508.5</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="26">
+      <c r="F6" s="39"/>
+      <c r="G6" s="22">
         <f t="shared" si="0"/>
         <v>535.26315789473688</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="22">
         <f t="shared" si="1"/>
         <v>0.10705263157894737</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="32"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="33" t="s">
+      <c r="A7" s="37"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="36">
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="25">
         <f>SUM(G3:G6)</f>
         <v>2293.1578947368425</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="25">
         <f>SUM(H3:H6)</f>
         <v>0.4586315789473685</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="21" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="38">
+        <v>5</v>
+      </c>
+      <c r="C8" s="38">
+        <v>1.3</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="21">
+        <v>1540</v>
+      </c>
+      <c r="F8" s="43">
+        <v>0.95</v>
+      </c>
+      <c r="G8" s="22">
+        <f>E8/$F$8</f>
+        <v>1621.0526315789475</v>
+      </c>
+      <c r="H8" s="22">
+        <f>(G8/$B$8)/1000</f>
+        <v>0.3242105263157895</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="46"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="21">
+        <v>5</v>
+      </c>
+      <c r="F9" s="44"/>
+      <c r="G9" s="22">
+        <f>E9/$F$8</f>
+        <v>5.2631578947368425</v>
+      </c>
+      <c r="H9" s="22">
+        <f>(G9/$B$8)/1000</f>
+        <v>1.0526315789473686E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="21">
+        <v>125</v>
+      </c>
+      <c r="F10" s="44"/>
+      <c r="G10" s="22">
+        <f>E10/$F$8</f>
+        <v>131.57894736842107</v>
+      </c>
+      <c r="H10" s="22">
+        <f>(G10/$B$8)/1000</f>
+        <v>2.6315789473684213E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="46"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="21">
+        <v>508.5</v>
+      </c>
+      <c r="F11" s="44"/>
+      <c r="G11" s="22">
+        <f>E11/$F$8</f>
+        <v>535.26315789473688</v>
+      </c>
+      <c r="H11" s="22">
+        <f>(G11/$B$8)/1000</f>
+        <v>0.10705263157894737</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="46"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="21">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F12" s="45"/>
+      <c r="G12" s="22">
+        <f>E12/$F$8</f>
+        <v>4.3684210526315796</v>
+      </c>
+      <c r="H12" s="22">
+        <f>(G12/$B$8)/1000</f>
+        <v>8.73684210526316E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="37"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="25">
+        <f>SUM(G8:G12)</f>
+        <v>2297.5263157894742</v>
+      </c>
+      <c r="H13" s="25">
+        <f>SUM(H8:H12)</f>
+        <v>0.45950526315789481</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="D16" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="E16" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" s="20" t="s">
+      <c r="G16" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="H16" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="H9" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="24">
-        <v>5</v>
-      </c>
-      <c r="C10" s="24">
-        <v>1.3</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="25">
-        <v>1540</v>
-      </c>
-      <c r="F10" s="37">
-        <v>0.95</v>
-      </c>
-      <c r="G10" s="26">
-        <f>E10/$F$10</f>
-        <v>1621.0526315789475</v>
-      </c>
-      <c r="H10" s="26">
-        <f>(G10/$B$10)/1000</f>
-        <v>0.3242105263157895</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="25">
-        <v>5</v>
-      </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="26">
-        <f t="shared" ref="G11:G14" si="2">E11/$F$10</f>
-        <v>5.2631578947368425</v>
-      </c>
-      <c r="H11" s="26">
-        <f t="shared" ref="H11:H14" si="3">(G11/$B$10)/1000</f>
-        <v>1.0526315789473686E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="25">
-        <v>125</v>
-      </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="26">
-        <f t="shared" si="2"/>
-        <v>131.57894736842107</v>
-      </c>
-      <c r="H12" s="26">
-        <f t="shared" si="3"/>
-        <v>2.6315789473684213E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="25">
-        <v>508.5</v>
-      </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="26">
-        <f t="shared" si="2"/>
-        <v>535.26315789473688</v>
-      </c>
-      <c r="H13" s="26">
-        <f t="shared" si="3"/>
-        <v>0.10705263157894737</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="25">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="26">
-        <f t="shared" si="2"/>
-        <v>4.3684210526315796</v>
-      </c>
-      <c r="H14" s="26">
-        <f t="shared" si="3"/>
-        <v>8.73684210526316E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="32"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="33" t="s">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="38">
+        <v>3.4</v>
+      </c>
+      <c r="C17" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="21">
+        <v>0</v>
+      </c>
+      <c r="F17" s="26">
+        <v>0.92</v>
+      </c>
+      <c r="G17" s="22">
+        <f>E17/$F$17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="22">
+        <f>(G17/$B$17)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="37"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="36">
-        <f>SUM(G10:G14)</f>
-        <v>2297.5263157894742</v>
-      </c>
-      <c r="H15" s="36">
-        <f>SUM(H10:H14)</f>
-        <v>0.45950526315789481</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="24">
-        <v>3.4</v>
-      </c>
-      <c r="C18" s="24">
+      <c r="E18" s="41"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="25">
+        <f>SUM(G17:G17)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="25">
+        <f>SUM(H17:H17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="38">
+        <v>3.3</v>
+      </c>
+      <c r="C19" s="38">
         <v>0.5</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D19" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="21">
+        <v>393</v>
+      </c>
+      <c r="F19" s="38">
+        <v>0.92</v>
+      </c>
+      <c r="G19" s="22">
+        <f>E19/$F$19</f>
+        <v>427.17391304347825</v>
+      </c>
+      <c r="H19" s="22">
+        <f>(G19/$B$19)/1000</f>
+        <v>0.12944664031620554</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="25">
-        <v>0</v>
-      </c>
-      <c r="F18" s="40">
-        <v>0.92</v>
-      </c>
-      <c r="G18" s="26">
-        <f>E18/$F$18</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="26">
-        <f>(G18/$B$18)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="32"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="36">
-        <f>SUM(G18:G18)</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="36">
-        <f>SUM(H18:H18)</f>
-        <v>0</v>
+      <c r="E20" s="21">
+        <v>264</v>
+      </c>
+      <c r="F20" s="47"/>
+      <c r="G20" s="22">
+        <f t="shared" ref="G20:G23" si="2">E20/$F$19</f>
+        <v>286.95652173913044</v>
+      </c>
+      <c r="H20" s="22">
+        <f t="shared" ref="H20:H23" si="3">(G20/$B$19)/1000</f>
+        <v>8.6956521739130432E-2</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="24">
-        <v>3.3</v>
-      </c>
-      <c r="C22" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="E22" s="25">
-        <v>393</v>
-      </c>
-      <c r="F22" s="24">
-        <v>0.92</v>
-      </c>
-      <c r="G22" s="26">
-        <f>E22/$F$22</f>
-        <v>427.17391304347825</v>
-      </c>
-      <c r="H22" s="26">
-        <f>(G22/$B$22)/1000</f>
-        <v>0.12944664031620554</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="25">
-        <v>264</v>
-      </c>
-      <c r="F23" s="29"/>
-      <c r="G23" s="26">
-        <f t="shared" ref="G23:G26" si="4">E23/$F$22</f>
-        <v>286.95652173913044</v>
-      </c>
-      <c r="H23" s="26">
-        <f t="shared" ref="H23:H26" si="5">(G23/$B$22)/1000</f>
-        <v>8.6956521739130432E-2</v>
-      </c>
-      <c r="I23" s="22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="E24" s="25">
+      <c r="A21" s="46"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="21">
         <f>(0.015*3.3)*1000</f>
         <v>49.499999999999993</v>
       </c>
-      <c r="F24" s="29"/>
-      <c r="G24" s="26">
-        <f t="shared" si="4"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="22">
+        <f t="shared" si="2"/>
         <v>53.804347826086946</v>
       </c>
-      <c r="H24" s="26">
-        <f t="shared" si="5"/>
+      <c r="H21" s="22">
+        <f t="shared" si="3"/>
         <v>1.6304347826086953E-2</v>
       </c>
     </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="46"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="21">
+        <v>363</v>
+      </c>
+      <c r="F22" s="47"/>
+      <c r="G22" s="22">
+        <f t="shared" si="2"/>
+        <v>394.56521739130432</v>
+      </c>
+      <c r="H22" s="22">
+        <f t="shared" si="3"/>
+        <v>0.11956521739130434</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="46"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="21">
+        <v>49.5</v>
+      </c>
+      <c r="F23" s="39"/>
+      <c r="G23" s="22">
+        <f t="shared" si="2"/>
+        <v>53.804347826086953</v>
+      </c>
+      <c r="H23" s="22">
+        <f t="shared" si="3"/>
+        <v>1.6304347826086956E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="37"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="41"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="25">
+        <f>SUM(G19:G23)</f>
+        <v>1216.304347826087</v>
+      </c>
+      <c r="H24" s="25">
+        <f>SUM(H19:H23)</f>
+        <v>0.36857707509881421</v>
+      </c>
+    </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="25">
-        <v>363</v>
-      </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="26">
-        <f t="shared" si="4"/>
-        <v>394.56521739130432</v>
-      </c>
-      <c r="H25" s="26">
-        <f t="shared" si="5"/>
-        <v>0.11956521739130434</v>
-      </c>
-      <c r="I25" s="22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="E26" s="25">
-        <v>49.5</v>
-      </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="26">
-        <f t="shared" si="4"/>
-        <v>53.804347826086953</v>
-      </c>
-      <c r="H26" s="26">
-        <f t="shared" si="5"/>
-        <v>1.6304347826086956E-2</v>
+      <c r="A25" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="38">
+        <v>1.8</v>
+      </c>
+      <c r="C25" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="21">
+        <v>207</v>
+      </c>
+      <c r="F25" s="26">
+        <v>0.84</v>
+      </c>
+      <c r="G25" s="22">
+        <f>E25/$F$25</f>
+        <v>246.42857142857144</v>
+      </c>
+      <c r="H25" s="22">
+        <f>(G25/$B$25)/1000</f>
+        <v>0.13690476190476189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="37"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="41"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="25">
+        <f>G25</f>
+        <v>246.42857142857144</v>
+      </c>
+      <c r="H26" s="25">
+        <f>H25</f>
+        <v>0.13690476190476189</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="32"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="33" t="s">
+      <c r="A27" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="38">
+        <v>1.8</v>
+      </c>
+      <c r="C27" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="21">
+        <v>2</v>
+      </c>
+      <c r="F27" s="38">
+        <v>0.84</v>
+      </c>
+      <c r="G27" s="25">
+        <f>E27/$F$25</f>
+        <v>2.3809523809523809</v>
+      </c>
+      <c r="H27" s="33">
+        <f>(G27/$B$25)/1000</f>
+        <v>1.3227513227513229E-3</v>
+      </c>
+      <c r="I27" s="28"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="46"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="21">
+        <v>0</v>
+      </c>
+      <c r="F28" s="39"/>
+      <c r="G28" s="22">
+        <f>E28/$F$25</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="22">
+        <f>(G28/$B$25)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="37"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36">
-        <f>SUM(G22:G26)</f>
-        <v>1216.304347826087</v>
-      </c>
-      <c r="H27" s="36">
-        <f>SUM(H22:H26)</f>
-        <v>0.36857707509881421</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="25">
+        <f>SUM(G27:G28)</f>
+        <v>2.3809523809523809</v>
+      </c>
+      <c r="H29" s="25">
+        <f>SUM(H27:H28)</f>
+        <v>1.3227513227513229E-3</v>
+      </c>
+      <c r="I29" s="21"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="38">
+        <v>5</v>
+      </c>
+      <c r="C30" s="38">
+        <v>2</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="21">
+        <v>275</v>
+      </c>
+      <c r="F30" s="38">
+        <v>1</v>
+      </c>
+      <c r="G30" s="22">
+        <f>E30/$F$30</f>
+        <v>275</v>
+      </c>
+      <c r="H30" s="30">
+        <f>(G30/$B$30)/1000</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="46"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="22">
+        <f t="shared" ref="G31" si="4">E31/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="22">
+        <f t="shared" ref="H31" si="5">(G31/$B$3)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="37"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="41"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="25">
+        <f>SUM(G30:G31)</f>
+        <v>275</v>
+      </c>
+      <c r="H32" s="25">
+        <f>SUM(H30:H31)</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="I32" s="31"/>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F37" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F38" s="21"/>
+      <c r="G38" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="H29" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="24">
-        <v>1.8</v>
-      </c>
-      <c r="C30" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="E30" s="25">
-        <v>207</v>
-      </c>
-      <c r="F30" s="40">
-        <v>0.84</v>
-      </c>
-      <c r="G30" s="26">
-        <f>E30/$F$30</f>
-        <v>246.42857142857144</v>
-      </c>
-      <c r="H30" s="26">
-        <f>(G30/$B$30)/1000</f>
-        <v>0.13690476190476189</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="32"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="33" t="s">
+      <c r="H38" s="32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F39" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="36">
-        <f>SUM(G30:G30)</f>
-        <v>246.42857142857144</v>
-      </c>
-      <c r="H31" s="36">
-        <f>SUM(H30:H30)</f>
-        <v>0.13690476190476189</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A33" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="I33" s="42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="24">
-        <v>1.8</v>
-      </c>
-      <c r="C34" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E34" s="25">
-        <v>2</v>
-      </c>
-      <c r="F34" s="24">
-        <v>0.84</v>
-      </c>
-      <c r="G34" s="36">
-        <f>E34/$F$30</f>
-        <v>2.3809523809523809</v>
-      </c>
-      <c r="H34" s="43">
-        <f>(G34/$B$30)/1000</f>
-        <v>1.3227513227513229E-3</v>
-      </c>
-      <c r="I34" s="42"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35" s="25">
-        <v>0</v>
-      </c>
-      <c r="F35" s="31"/>
-      <c r="G35" s="26">
-        <f>E35/$F$30</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="26">
-        <f>(G35/$B$30)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="32"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="36">
-        <f>SUM(G35:G35)</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="36">
-        <f>SUM(H35:H35)</f>
-        <v>0</v>
-      </c>
-      <c r="I36" s="25"/>
-    </row>
-    <row r="38" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F38" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="H38" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="I38" s="42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" s="24">
-        <v>5</v>
-      </c>
-      <c r="C39" s="24">
-        <v>2</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="E39" s="25">
-        <v>275</v>
-      </c>
-      <c r="F39" s="24">
-        <v>1</v>
-      </c>
-      <c r="G39" s="26">
-        <f>E39/$F$39</f>
-        <v>275</v>
-      </c>
-      <c r="H39" s="45">
-        <f>(G39/$B$39)/1000</f>
-        <v>5.5E-2</v>
-      </c>
-      <c r="I39" s="46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="28"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="E40" s="25"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="26">
-        <f t="shared" ref="G40" si="6">E40/$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="H40" s="26">
-        <f t="shared" ref="H40" si="7">(G40/$B$3)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="46" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="32"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="E41" s="34"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="36">
-        <f>SUM(G39:G40)</f>
-        <v>275</v>
-      </c>
-      <c r="H41" s="36">
-        <f>SUM(H39:H40)</f>
-        <v>5.5E-2</v>
-      </c>
-      <c r="I41" s="46"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F46" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F47" s="25"/>
-      <c r="G47" s="48" t="s">
-        <v>117</v>
-      </c>
-      <c r="H47" s="48" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F48" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="G48" s="26">
-        <f>SUM(G15,G19,G27,G31,G41)</f>
+      <c r="G39" s="22">
+        <f>SUM(G13,G18,G24,G26,G32)</f>
         <v>4035.2592350441328</v>
       </c>
-      <c r="H48" s="25">
-        <f>(G48/5)/1000</f>
+      <c r="H39" s="21">
+        <f>(G39/5)/1000</f>
         <v>0.80705184700882659</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="F19:F23"/>
+    <mergeCell ref="D24:F24"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="F3:F6"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="G26:H26" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished power budget section of prelim report
</commit_message>
<xml_diff>
--- a/DOCS/Power_Budget.xlsx
+++ b/DOCS/Power_Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\ETS\Hivers 2020\ELE682\ele682\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8662FDC0-6B43-4E21-BBAF-01775575C4C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60029F02-F9E1-4657-84D7-9C65406D5C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="7448" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="7448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OSD335-X Power Rails" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="125">
   <si>
     <t>OSD335x-SM Family Power Budget</t>
   </si>
@@ -400,9 +400,6 @@
     <t>Efficacité*</t>
   </si>
   <si>
-    <t>PUISSANCE CONSOMMÉE MAXIMALE</t>
-  </si>
-  <si>
     <t>Puissance (mW)</t>
   </si>
   <si>
@@ -430,6 +427,15 @@
   </si>
   <si>
     <t>Alimentation</t>
+  </si>
+  <si>
+    <t>Consommation totale</t>
+  </si>
+  <si>
+    <t>Disponible selon l'alimentation</t>
+  </si>
+  <si>
+    <t>Différence</t>
   </si>
 </sst>
 </file>
@@ -639,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -738,6 +744,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -759,6 +768,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -768,13 +783,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1108,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:G7"/>
     </sheetView>
   </sheetViews>
@@ -2065,16 +2086,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B18:G18"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2083,10 +2104,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:I39"/>
+  <dimension ref="A2:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38:H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
@@ -2098,7 +2119,7 @@
     <col min="5" max="5" width="14.46484375" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.59765625" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.46484375" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.59765625" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="130.3984375" style="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="42.86328125" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.1328125" style="20"/>
@@ -2106,7 +2127,7 @@
   <sheetData>
     <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>110</v>
@@ -2118,26 +2139,26 @@
         <v>112</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>113</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="39">
         <v>5</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="39">
         <v>2</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -2146,7 +2167,7 @@
       <c r="E3" s="21">
         <v>1540</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="39">
         <v>0.95</v>
       </c>
       <c r="G3" s="22">
@@ -2162,16 +2183,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="21" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="21">
         <v>5</v>
       </c>
-      <c r="F4" s="47"/>
+      <c r="F4" s="45"/>
       <c r="G4" s="22">
         <f t="shared" ref="G4:G6" si="0">E4/$F$3</f>
         <v>5.2631578947368425</v>
@@ -2183,16 +2204,16 @@
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="21" t="s">
         <v>71</v>
       </c>
       <c r="E5" s="21">
         <v>125</v>
       </c>
-      <c r="F5" s="47"/>
+      <c r="F5" s="45"/>
       <c r="G5" s="22">
         <f t="shared" si="0"/>
         <v>131.57894736842107</v>
@@ -2203,16 +2224,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="46"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="21" t="s">
         <v>88</v>
       </c>
       <c r="E6" s="21">
         <v>508.5</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="22">
         <f t="shared" si="0"/>
         <v>535.26315789473688</v>
@@ -2223,14 +2244,14 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="37"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="25">
         <f>SUM(G3:G6)</f>
         <v>2293.1578947368425</v>
@@ -2241,13 +2262,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="39">
         <v>5</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="39">
         <v>1.3</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2256,7 +2277,7 @@
       <c r="E8" s="21">
         <v>1540</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="46">
         <v>0.95</v>
       </c>
       <c r="G8" s="22">
@@ -2269,16 +2290,16 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="46"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="21" t="s">
         <v>65</v>
       </c>
       <c r="E9" s="21">
         <v>5</v>
       </c>
-      <c r="F9" s="44"/>
+      <c r="F9" s="47"/>
       <c r="G9" s="22">
         <f>E9/$F$8</f>
         <v>5.2631578947368425</v>
@@ -2289,16 +2310,16 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="46"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="21" t="s">
         <v>71</v>
       </c>
       <c r="E10" s="21">
         <v>125</v>
       </c>
-      <c r="F10" s="44"/>
+      <c r="F10" s="47"/>
       <c r="G10" s="22">
         <f>E10/$F$8</f>
         <v>131.57894736842107</v>
@@ -2309,16 +2330,16 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="46"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="21" t="s">
         <v>88</v>
       </c>
       <c r="E11" s="21">
         <v>508.5</v>
       </c>
-      <c r="F11" s="44"/>
+      <c r="F11" s="47"/>
       <c r="G11" s="22">
         <f>E11/$F$8</f>
         <v>535.26315789473688</v>
@@ -2329,16 +2350,16 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="46"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="21" t="s">
         <v>106</v>
       </c>
       <c r="E12" s="21">
         <v>4.1500000000000004</v>
       </c>
-      <c r="F12" s="45"/>
+      <c r="F12" s="48"/>
       <c r="G12" s="22">
         <f>E12/$F$8</f>
         <v>4.3684210526315796</v>
@@ -2349,14 +2370,14 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="40" t="s">
+      <c r="A13" s="38"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
       <c r="G13" s="25">
         <f>SUM(G8:G12)</f>
         <v>2297.5263157894742</v>
@@ -2368,7 +2389,7 @@
     </row>
     <row r="16" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>110</v>
@@ -2380,26 +2401,26 @@
         <v>112</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>113</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="38">
+      <c r="B17" s="39">
         <v>3.4</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="39">
         <v>0.5</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -2424,14 +2445,14 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="37"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="41"/>
-      <c r="F18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="43"/>
       <c r="G18" s="25">
         <f>SUM(G17:G17)</f>
         <v>0</v>
@@ -2442,13 +2463,13 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="38">
+      <c r="B19" s="39">
         <v>3.3</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="39">
         <v>0.5</v>
       </c>
       <c r="D19" s="21" t="s">
@@ -2457,7 +2478,7 @@
       <c r="E19" s="21">
         <v>393</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="39">
         <v>0.92</v>
       </c>
       <c r="G19" s="22">
@@ -2470,16 +2491,16 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="46"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="21" t="s">
         <v>52</v>
       </c>
       <c r="E20" s="21">
         <v>264</v>
       </c>
-      <c r="F20" s="47"/>
+      <c r="F20" s="45"/>
       <c r="G20" s="22">
         <f t="shared" ref="G20:G23" si="2">E20/$F$19</f>
         <v>286.95652173913044</v>
@@ -2493,17 +2514,17 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="46"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" s="21">
         <f>(0.015*3.3)*1000</f>
         <v>49.499999999999993</v>
       </c>
-      <c r="F21" s="47"/>
+      <c r="F21" s="45"/>
       <c r="G21" s="22">
         <f t="shared" si="2"/>
         <v>53.804347826086946</v>
@@ -2514,16 +2535,16 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="46"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
       <c r="D22" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E22" s="21">
         <v>363</v>
       </c>
-      <c r="F22" s="47"/>
+      <c r="F22" s="45"/>
       <c r="G22" s="22">
         <f t="shared" si="2"/>
         <v>394.56521739130432</v>
@@ -2537,16 +2558,16 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="46"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" s="21">
         <v>49.5</v>
       </c>
-      <c r="F23" s="39"/>
+      <c r="F23" s="40"/>
       <c r="G23" s="22">
         <f t="shared" si="2"/>
         <v>53.804347826086953</v>
@@ -2557,14 +2578,14 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="37"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40" t="s">
+      <c r="A24" s="38"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
       <c r="G24" s="25">
         <f>SUM(G19:G23)</f>
         <v>1216.304347826087</v>
@@ -2575,13 +2596,13 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="38">
+      <c r="B25" s="39">
         <v>1.8</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="39">
         <v>0.1</v>
       </c>
       <c r="D25" s="21" t="s">
@@ -2603,14 +2624,14 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="37"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="40" t="s">
+      <c r="A26" s="38"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="43"/>
       <c r="G26" s="25">
         <f>G25</f>
         <v>246.42857142857144</v>
@@ -2621,13 +2642,13 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="38">
+      <c r="B27" s="39">
         <v>1.8</v>
       </c>
-      <c r="C27" s="38">
+      <c r="C27" s="39">
         <v>0.1</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -2636,7 +2657,7 @@
       <c r="E27" s="21">
         <v>2</v>
       </c>
-      <c r="F27" s="38">
+      <c r="F27" s="39">
         <v>0.84</v>
       </c>
       <c r="G27" s="25">
@@ -2650,16 +2671,16 @@
       <c r="I27" s="28"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="46"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
+      <c r="A28" s="44"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
       <c r="D28" s="21" t="s">
         <v>98</v>
       </c>
       <c r="E28" s="21">
         <v>0</v>
       </c>
-      <c r="F28" s="39"/>
+      <c r="F28" s="40"/>
       <c r="G28" s="22">
         <f>E28/$F$25</f>
         <v>0</v>
@@ -2673,14 +2694,14 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="37"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="40" t="s">
+      <c r="A29" s="38"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="43"/>
       <c r="G29" s="25">
         <f>SUM(G27:G28)</f>
         <v>2.3809523809523809</v>
@@ -2692,13 +2713,13 @@
       <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="38">
+      <c r="B30" s="39">
         <v>5</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C30" s="39">
         <v>2</v>
       </c>
       <c r="D30" s="21" t="s">
@@ -2707,7 +2728,7 @@
       <c r="E30" s="21">
         <v>275</v>
       </c>
-      <c r="F30" s="38">
+      <c r="F30" s="39">
         <v>1</v>
       </c>
       <c r="G30" s="22">
@@ -2723,14 +2744,14 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="46"/>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
       <c r="D31" s="21" t="s">
         <v>107</v>
       </c>
       <c r="E31" s="21"/>
-      <c r="F31" s="47"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="22">
         <f t="shared" ref="G31" si="4">E31/$F$3</f>
         <v>0</v>
@@ -2744,14 +2765,14 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="37"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="40" t="s">
+      <c r="A32" s="38"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="E32" s="41"/>
-      <c r="F32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="25">
         <f>SUM(G30:G31)</f>
         <v>275</v>
@@ -2763,36 +2784,99 @@
       <c r="I32" s="31"/>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F37" s="48" t="s">
+      <c r="F37" s="51"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F38" s="53"/>
+      <c r="G38" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-    </row>
-    <row r="38" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F38" s="21"/>
-      <c r="G38" s="32" t="s">
+      <c r="H38" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="H38" s="32" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F39" s="32" t="s">
-        <v>89</v>
+      <c r="F39" s="49" t="s">
+        <v>123</v>
       </c>
       <c r="G39" s="22">
+        <v>10000</v>
+      </c>
+      <c r="H39" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F40" s="49"/>
+      <c r="G40" s="22">
+        <v>6500</v>
+      </c>
+      <c r="H40" s="21">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="41" spans="6:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="F41" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="G41" s="22">
         <f>SUM(G13,G18,G24,G26,G32)</f>
         <v>4035.2592350441328</v>
       </c>
-      <c r="H39" s="21">
-        <f>(G39/5)/1000</f>
+      <c r="H41" s="22">
+        <f>(G41/5)/1000</f>
         <v>0.80705184700882659</v>
       </c>
     </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F42" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="G42" s="22">
+        <f>G39-G41</f>
+        <v>5964.7407649558672</v>
+      </c>
+      <c r="H42" s="22">
+        <f>H39-H41</f>
+        <v>1.1929481529911734</v>
+      </c>
+    </row>
+    <row r="43" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F43" s="49"/>
+      <c r="G43" s="22">
+        <f>G40-G41</f>
+        <v>2464.7407649558672</v>
+      </c>
+      <c r="H43" s="22">
+        <f>H40-H41</f>
+        <v>0.49294815299117345</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="36">
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="F19:F23"/>
+    <mergeCell ref="D24:F24"/>
     <mergeCell ref="F37:H37"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
@@ -2808,25 +2892,6 @@
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="C27:C29"/>
     <mergeCell ref="F27:F28"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="F19:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="D13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>